<commit_message>
Ik denk dat het werkt?
</commit_message>
<xml_diff>
--- a/Code/Estimated Data/demand_2026_matrix.xlsx
+++ b/Code/Estimated Data/demand_2026_matrix.xlsx
@@ -545,61 +545,61 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>3.419074076731379</v>
+        <v>1045.501704723878</v>
       </c>
       <c r="D2" t="n">
-        <v>2.153226750020909</v>
+        <v>681.5869269208697</v>
       </c>
       <c r="E2" t="n">
-        <v>1.59562930638585</v>
+        <v>338.9306982050842</v>
       </c>
       <c r="F2" t="n">
-        <v>2.400089917580012</v>
+        <v>284.4217910886661</v>
       </c>
       <c r="G2" t="n">
-        <v>1.551116481526844</v>
+        <v>214.5323724753912</v>
       </c>
       <c r="H2" t="n">
-        <v>2.15868193994416</v>
+        <v>321.7211544727224</v>
       </c>
       <c r="I2" t="n">
-        <v>2.192445911345847</v>
+        <v>234.0632048431902</v>
       </c>
       <c r="J2" t="n">
-        <v>2.878426991170778</v>
+        <v>708.6677278466523</v>
       </c>
       <c r="K2" t="n">
-        <v>1.47356778430757</v>
+        <v>166.1826814839588</v>
       </c>
       <c r="L2" t="n">
-        <v>0.5438198426873661</v>
+        <v>73.24146606853961</v>
       </c>
       <c r="M2" t="n">
-        <v>3.922967561809019</v>
+        <v>515.6608006389828</v>
       </c>
       <c r="N2" t="n">
-        <v>0.9458255215543545</v>
+        <v>97.0434555773428</v>
       </c>
       <c r="O2" t="n">
-        <v>1.087597558904144</v>
+        <v>134.9474873993719</v>
       </c>
       <c r="P2" t="n">
-        <v>1.333036089377373</v>
+        <v>346.9043594620259</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.8136410108990793</v>
+        <v>80.81337308968041</v>
       </c>
       <c r="R2" t="n">
-        <v>0.180914330084948</v>
+        <v>19.58346306481534</v>
       </c>
       <c r="S2" t="n">
-        <v>0.3810106783015563</v>
+        <v>45.67233265707532</v>
       </c>
       <c r="T2" t="n">
-        <v>0.7633374454492508</v>
+        <v>83.14824786265031</v>
       </c>
       <c r="U2" t="n">
-        <v>0.1650575341562291</v>
+        <v>19.55206696407565</v>
       </c>
     </row>
     <row r="3">
@@ -609,64 +609,64 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3.419074076731379</v>
+        <v>1045.501704723878</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0.761478607948153</v>
+        <v>281.8681414562378</v>
       </c>
       <c r="E3" t="n">
-        <v>0.6575086815580207</v>
+        <v>227.6403930034599</v>
       </c>
       <c r="F3" t="n">
-        <v>0.9177615587365008</v>
+        <v>150.7028303599278</v>
       </c>
       <c r="G3" t="n">
-        <v>0.6204977054491737</v>
+        <v>131.1590154118439</v>
       </c>
       <c r="H3" t="n">
-        <v>0.8733176109819948</v>
+        <v>203.8393959382139</v>
       </c>
       <c r="I3" t="n">
-        <v>0.8715019607159229</v>
+        <v>140.2477869647435</v>
       </c>
       <c r="J3" t="n">
-        <v>0.8629930405265916</v>
+        <v>173.5791897611845</v>
       </c>
       <c r="K3" t="n">
-        <v>0.524917649163571</v>
+        <v>70.32530360250405</v>
       </c>
       <c r="L3" t="n">
-        <v>0.2013106974107253</v>
+        <v>35.012482745424</v>
       </c>
       <c r="M3" t="n">
-        <v>1.474978535206565</v>
+        <v>258.9815891272129</v>
       </c>
       <c r="N3" t="n">
-        <v>0.3398728936307667</v>
+        <v>42.21780754175937</v>
       </c>
       <c r="O3" t="n">
-        <v>0.4065264346844761</v>
+        <v>66.52426997853188</v>
       </c>
       <c r="P3" t="n">
-        <v>0.4093730667284161</v>
+        <v>91.69208996276853</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.3080831854734076</v>
+        <v>41.50563265940433</v>
       </c>
       <c r="R3" t="n">
-        <v>0.06847852484732431</v>
+        <v>10.04675171482197</v>
       </c>
       <c r="S3" t="n">
-        <v>0.1304450846752479</v>
+        <v>17.04225531138226</v>
       </c>
       <c r="T3" t="n">
-        <v>0.2971229088388304</v>
+        <v>46.61109119060586</v>
       </c>
       <c r="U3" t="n">
-        <v>0.06024339699417602</v>
+        <v>8.936981748599937</v>
       </c>
     </row>
     <row r="4">
@@ -676,64 +676,64 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2.153226750020909</v>
+        <v>681.5869269208697</v>
       </c>
       <c r="C4" t="n">
-        <v>0.761478607948153</v>
+        <v>281.8681414562378</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0.4535444592751538</v>
+        <v>198.0844625790089</v>
       </c>
       <c r="F4" t="n">
-        <v>0.5306128862042053</v>
+        <v>74.90964325441705</v>
       </c>
       <c r="G4" t="n">
-        <v>0.352465225839925</v>
+        <v>61.6425790025206</v>
       </c>
       <c r="H4" t="n">
-        <v>0.5672293024866779</v>
+        <v>146.555946650177</v>
       </c>
       <c r="I4" t="n">
-        <v>0.5306651402483423</v>
+        <v>82.16593044605925</v>
       </c>
       <c r="J4" t="n">
-        <v>0.5642502252728027</v>
+        <v>127.4504865588624</v>
       </c>
       <c r="K4" t="n">
-        <v>0.3729256446322989</v>
+        <v>67.19736812210172</v>
       </c>
       <c r="L4" t="n">
-        <v>0.1199422967424666</v>
+        <v>19.14500564717642</v>
       </c>
       <c r="M4" t="n">
-        <v>1.082787059394819</v>
+        <v>274.5571331803888</v>
       </c>
       <c r="N4" t="n">
-        <v>0.2358105937030529</v>
+        <v>37.42108833563172</v>
       </c>
       <c r="O4" t="n">
-        <v>0.2799740315382225</v>
+        <v>57.59628932726799</v>
       </c>
       <c r="P4" t="n">
-        <v>0.2884292850508153</v>
+        <v>85.33341443088079</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.2008518829345858</v>
+        <v>30.19710947158296</v>
       </c>
       <c r="R4" t="n">
-        <v>0.04353084885517617</v>
+        <v>6.746902998405186</v>
       </c>
       <c r="S4" t="n">
-        <v>0.08674531588967811</v>
+        <v>13.20371190782591</v>
       </c>
       <c r="T4" t="n">
-        <v>0.1823572814217435</v>
+        <v>28.00138615746715</v>
       </c>
       <c r="U4" t="n">
-        <v>0.03699143648735424</v>
+        <v>5.376883589600534</v>
       </c>
     </row>
     <row r="5">
@@ -743,64 +743,64 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1.59562930638585</v>
+        <v>338.9306982050842</v>
       </c>
       <c r="C5" t="n">
-        <v>0.6575086815580207</v>
+        <v>227.6403930034599</v>
       </c>
       <c r="D5" t="n">
-        <v>0.4535444592751538</v>
+        <v>198.0844625790089</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>0.4815969460344361</v>
+        <v>70.86788499495998</v>
       </c>
       <c r="G5" t="n">
-        <v>0.3309432120613822</v>
+        <v>64.94077468183021</v>
       </c>
       <c r="H5" t="n">
-        <v>0.6691581562664916</v>
+        <v>318.4723755706087</v>
       </c>
       <c r="I5" t="n">
-        <v>0.5290168959373047</v>
+        <v>104.6726220019602</v>
       </c>
       <c r="J5" t="n">
-        <v>0.4473697029083934</v>
+        <v>78.52939523939308</v>
       </c>
       <c r="K5" t="n">
-        <v>0.3286729019159626</v>
+        <v>57.91326073029241</v>
       </c>
       <c r="L5" t="n">
-        <v>0.1073335559929054</v>
+        <v>17.31743132701527</v>
       </c>
       <c r="M5" t="n">
-        <v>1.075584263980863</v>
+        <v>345.8321373052493</v>
       </c>
       <c r="N5" t="n">
-        <v>0.2113039957247282</v>
+        <v>33.9928814565047</v>
       </c>
       <c r="O5" t="n">
-        <v>0.2700702552886041</v>
+        <v>66.10139166955875</v>
       </c>
       <c r="P5" t="n">
-        <v>0.2234972351990707</v>
+        <v>48.88911038034519</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.1938515518072781</v>
+        <v>34.71561414850142</v>
       </c>
       <c r="R5" t="n">
-        <v>0.04133862966660069</v>
+        <v>7.368040317792743</v>
       </c>
       <c r="S5" t="n">
-        <v>0.07378240204932295</v>
+        <v>10.16635119976261</v>
       </c>
       <c r="T5" t="n">
-        <v>0.1765718719894737</v>
+        <v>32.52336967366866</v>
       </c>
       <c r="U5" t="n">
-        <v>0.03305904368634398</v>
+        <v>4.843259864789729</v>
       </c>
     </row>
     <row r="6">
@@ -810,64 +810,64 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2.400089917580012</v>
+        <v>284.4217910886661</v>
       </c>
       <c r="C6" t="n">
-        <v>0.9177615587365008</v>
+        <v>150.7028303599278</v>
       </c>
       <c r="D6" t="n">
-        <v>0.5306128862042053</v>
+        <v>74.90964325441705</v>
       </c>
       <c r="E6" t="n">
-        <v>0.4815969460344361</v>
+        <v>70.86788499495998</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>0.8180163819857508</v>
+        <v>263.3734819180988</v>
       </c>
       <c r="H6" t="n">
-        <v>0.7244457062064737</v>
+        <v>94.17366998159903</v>
       </c>
       <c r="I6" t="n">
-        <v>0.8859042831941888</v>
+        <v>123.4698193430533</v>
       </c>
       <c r="J6" t="n">
-        <v>0.7585378235887275</v>
+        <v>96.35336660463844</v>
       </c>
       <c r="K6" t="n">
-        <v>0.4760095217432692</v>
+        <v>43.09960859506008</v>
       </c>
       <c r="L6" t="n">
-        <v>0.3121623755544702</v>
+        <v>117.6479300738739</v>
       </c>
       <c r="M6" t="n">
-        <v>1.22675696107325</v>
+        <v>120.6489700032122</v>
       </c>
       <c r="N6" t="n">
-        <v>0.3170686428569893</v>
+        <v>28.30803808649734</v>
       </c>
       <c r="O6" t="n">
-        <v>0.3685296416461688</v>
+        <v>40.72819249184865</v>
       </c>
       <c r="P6" t="n">
-        <v>0.3516959041426887</v>
+        <v>47.34025871597547</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.3032074755595441</v>
+        <v>32.97758148196699</v>
       </c>
       <c r="R6" t="n">
-        <v>0.07238586604615192</v>
+        <v>10.01269413604668</v>
       </c>
       <c r="S6" t="n">
-        <v>0.1296521049734978</v>
+        <v>13.97056726190151</v>
       </c>
       <c r="T6" t="n">
-        <v>0.3231051337461743</v>
+        <v>50.82230770753425</v>
       </c>
       <c r="U6" t="n">
-        <v>0.07756568373691207</v>
+        <v>16.65009348587779</v>
       </c>
     </row>
     <row r="7">
@@ -877,64 +877,64 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1.551116481526844</v>
+        <v>214.5323724753912</v>
       </c>
       <c r="C7" t="n">
-        <v>0.6204977054491737</v>
+        <v>131.1590154118439</v>
       </c>
       <c r="D7" t="n">
-        <v>0.352465225839925</v>
+        <v>61.6425790025206</v>
       </c>
       <c r="E7" t="n">
-        <v>0.3309432120613822</v>
+        <v>64.94077468183021</v>
       </c>
       <c r="F7" t="n">
-        <v>0.8180163819857508</v>
+        <v>263.3734819180988</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>0.5064310923873764</v>
+        <v>91.11941768350989</v>
       </c>
       <c r="I7" t="n">
-        <v>0.6490691388726352</v>
+        <v>138.6482841535388</v>
       </c>
       <c r="J7" t="n">
-        <v>0.4733170862062743</v>
+        <v>65.02077305932224</v>
       </c>
       <c r="K7" t="n">
-        <v>0.3112655816447387</v>
+        <v>33.74232519574387</v>
       </c>
       <c r="L7" t="n">
-        <v>0.1566591624062391</v>
+        <v>39.78473003089972</v>
       </c>
       <c r="M7" t="n">
-        <v>0.8265860502035145</v>
+        <v>103.8732221004126</v>
       </c>
       <c r="N7" t="n">
-        <v>0.2071947498413253</v>
+        <v>22.11523703683941</v>
       </c>
       <c r="O7" t="n">
-        <v>0.2474484073603518</v>
+        <v>34.67867633617257</v>
       </c>
       <c r="P7" t="n">
-        <v>0.2230132641965453</v>
+        <v>33.61877907668124</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.2050814867229246</v>
+        <v>28.7378668712236</v>
       </c>
       <c r="R7" t="n">
-        <v>0.04863836399039231</v>
+        <v>8.544977673146949</v>
       </c>
       <c r="S7" t="n">
-        <v>0.08064961509683467</v>
+        <v>9.334913483324714</v>
       </c>
       <c r="T7" t="n">
-        <v>0.229856606740604</v>
+        <v>51.98011656689501</v>
       </c>
       <c r="U7" t="n">
-        <v>0.04439523944085714</v>
+        <v>8.543440697881632</v>
       </c>
     </row>
     <row r="8">
@@ -944,64 +944,64 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2.15868193994416</v>
+        <v>321.7211544727224</v>
       </c>
       <c r="C8" t="n">
-        <v>0.8733176109819948</v>
+        <v>203.8393959382139</v>
       </c>
       <c r="D8" t="n">
-        <v>0.5672293024866779</v>
+        <v>146.555946650177</v>
       </c>
       <c r="E8" t="n">
-        <v>0.6691581562664916</v>
+        <v>318.4723755706087</v>
       </c>
       <c r="F8" t="n">
-        <v>0.7244457062064737</v>
+        <v>94.17366998159903</v>
       </c>
       <c r="G8" t="n">
-        <v>0.5064310923873764</v>
+        <v>91.11941768350989</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>0.88841680208732</v>
+        <v>197.2448578266715</v>
       </c>
       <c r="J8" t="n">
-        <v>0.6312113032282947</v>
+        <v>85.17096310026463</v>
       </c>
       <c r="K8" t="n">
-        <v>0.4905648366225033</v>
+        <v>75.07698709470658</v>
       </c>
       <c r="L8" t="n">
-        <v>0.1611511710801652</v>
+        <v>22.87438245754333</v>
       </c>
       <c r="M8" t="n">
-        <v>1.588590084643201</v>
+        <v>433.6251574482413</v>
       </c>
       <c r="N8" t="n">
-        <v>0.3208769405714093</v>
+        <v>46.54788929841322</v>
       </c>
       <c r="O8" t="n">
-        <v>0.4339113337923615</v>
+        <v>108.2458795829952</v>
       </c>
       <c r="P8" t="n">
-        <v>0.3139062177154358</v>
+        <v>52.26246126117292</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.3190318309550865</v>
+        <v>61.35373183100276</v>
       </c>
       <c r="R8" t="n">
-        <v>0.06661587561197994</v>
+        <v>12.18057984799809</v>
       </c>
       <c r="S8" t="n">
-        <v>0.108640028769557</v>
+        <v>12.62393291365497</v>
       </c>
       <c r="T8" t="n">
-        <v>0.2878116514519349</v>
+        <v>55.75196439482628</v>
       </c>
       <c r="U8" t="n">
-        <v>0.04994393323830284</v>
+        <v>6.524543999018621</v>
       </c>
     </row>
     <row r="9">
@@ -1011,64 +1011,64 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2.192445911345847</v>
+        <v>234.0632048431902</v>
       </c>
       <c r="C9" t="n">
-        <v>0.8715019607159229</v>
+        <v>140.2477869647435</v>
       </c>
       <c r="D9" t="n">
-        <v>0.5306651402483423</v>
+        <v>82.16593044605925</v>
       </c>
       <c r="E9" t="n">
-        <v>0.5290168959373047</v>
+        <v>104.6726220019602</v>
       </c>
       <c r="F9" t="n">
-        <v>0.8859042831941888</v>
+        <v>123.4698193430533</v>
       </c>
       <c r="G9" t="n">
-        <v>0.6490691388726352</v>
+        <v>138.6482841535388</v>
       </c>
       <c r="H9" t="n">
-        <v>0.88841680208732</v>
+        <v>197.2448578266715</v>
       </c>
       <c r="I9" t="n">
         <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>0.6669484373102005</v>
+        <v>70.24707606986435</v>
       </c>
       <c r="K9" t="n">
-        <v>0.497984270719071</v>
+        <v>54.53299256456867</v>
       </c>
       <c r="L9" t="n">
-        <v>0.1942260742168652</v>
+        <v>28.64022165003827</v>
       </c>
       <c r="M9" t="n">
-        <v>1.366377798739836</v>
+        <v>186.2181677820286</v>
       </c>
       <c r="N9" t="n">
-        <v>0.3346350200303586</v>
+        <v>36.83037390456204</v>
       </c>
       <c r="O9" t="n">
-        <v>0.4249074442317431</v>
+        <v>70.14576502997072</v>
       </c>
       <c r="P9" t="n">
-        <v>0.3246362246489543</v>
+        <v>40.2683498525008</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.3756539200634958</v>
+        <v>71.34584298681415</v>
       </c>
       <c r="R9" t="n">
-        <v>0.08695661177093397</v>
+        <v>19.6426930247282</v>
       </c>
       <c r="S9" t="n">
-        <v>0.118832145734371</v>
+        <v>11.61964733545398</v>
       </c>
       <c r="T9" t="n">
-        <v>0.4753837331846074</v>
+        <v>189.6654677537916</v>
       </c>
       <c r="U9" t="n">
-        <v>0.06011014164273937</v>
+        <v>8.132898353418625</v>
       </c>
     </row>
     <row r="10">
@@ -1078,64 +1078,64 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2.878426991170778</v>
+        <v>708.6677278466523</v>
       </c>
       <c r="C10" t="n">
-        <v>0.8629930405265916</v>
+        <v>173.5791897611845</v>
       </c>
       <c r="D10" t="n">
-        <v>0.5642502252728027</v>
+        <v>127.4504865588624</v>
       </c>
       <c r="E10" t="n">
-        <v>0.4473697029083934</v>
+        <v>78.52939523939308</v>
       </c>
       <c r="F10" t="n">
-        <v>0.7585378235887275</v>
+        <v>96.35336660463844</v>
       </c>
       <c r="G10" t="n">
-        <v>0.4733170862062743</v>
+        <v>65.02077305932224</v>
       </c>
       <c r="H10" t="n">
-        <v>0.6312113032282947</v>
+        <v>85.17096310026463</v>
       </c>
       <c r="I10" t="n">
-        <v>0.6669484373102005</v>
+        <v>70.24707606986435</v>
       </c>
       <c r="J10" t="n">
         <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>0.4736019551735381</v>
+        <v>59.37777136911156</v>
       </c>
       <c r="L10" t="n">
-        <v>0.1781536440331379</v>
+        <v>27.80414180236518</v>
       </c>
       <c r="M10" t="n">
-        <v>1.170812233809938</v>
+        <v>145.6673403629809</v>
       </c>
       <c r="N10" t="n">
-        <v>0.3054930133291014</v>
+        <v>35.2219920856481</v>
       </c>
       <c r="O10" t="n">
-        <v>0.336527149460932</v>
+        <v>42.74594548528522</v>
       </c>
       <c r="P10" t="n">
-        <v>0.5190083083319154</v>
+        <v>227.7328192760707</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.25454816801986</v>
+        <v>26.50887789075907</v>
       </c>
       <c r="R10" t="n">
-        <v>0.05720500012878239</v>
+        <v>6.644521418341258</v>
       </c>
       <c r="S10" t="n">
-        <v>0.1374899798657545</v>
+        <v>23.56154612713247</v>
       </c>
       <c r="T10" t="n">
-        <v>0.2366168888707608</v>
+        <v>26.48796839735648</v>
       </c>
       <c r="U10" t="n">
-        <v>0.055134499732434</v>
+        <v>7.894816085537324</v>
       </c>
     </row>
     <row r="11">
@@ -1145,64 +1145,64 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1.47356778430757</v>
+        <v>166.1826814839588</v>
       </c>
       <c r="C11" t="n">
-        <v>0.524917649163571</v>
+        <v>70.32530360250405</v>
       </c>
       <c r="D11" t="n">
-        <v>0.3729256446322989</v>
+        <v>67.19736812210172</v>
       </c>
       <c r="E11" t="n">
-        <v>0.3286729019159626</v>
+        <v>57.91326073029241</v>
       </c>
       <c r="F11" t="n">
-        <v>0.4760095217432692</v>
+        <v>43.09960859506008</v>
       </c>
       <c r="G11" t="n">
-        <v>0.3112655816447387</v>
+        <v>33.74232519574387</v>
       </c>
       <c r="H11" t="n">
-        <v>0.4905648366225033</v>
+        <v>75.07698709470658</v>
       </c>
       <c r="I11" t="n">
-        <v>0.497984270719071</v>
+        <v>54.53299256456867</v>
       </c>
       <c r="J11" t="n">
-        <v>0.4736019551735381</v>
+        <v>59.37777136911156</v>
       </c>
       <c r="K11" t="n">
         <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>0.1110292504346903</v>
+        <v>12.16785725437241</v>
       </c>
       <c r="M11" t="n">
-        <v>1.041523263089528</v>
+        <v>197.0772999840456</v>
       </c>
       <c r="N11" t="n">
-        <v>0.4059094980144862</v>
+        <v>170.1240629777096</v>
       </c>
       <c r="O11" t="n">
-        <v>0.3332656445419659</v>
+        <v>81.27188082777515</v>
       </c>
       <c r="P11" t="n">
-        <v>0.2495374644451636</v>
+        <v>43.76487725055504</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.2200571445989937</v>
+        <v>32.75546275286384</v>
       </c>
       <c r="R11" t="n">
-        <v>0.04586044398245579</v>
+        <v>6.463137570691012</v>
       </c>
       <c r="S11" t="n">
-        <v>0.09309003696221417</v>
+        <v>13.41097756165878</v>
       </c>
       <c r="T11" t="n">
-        <v>0.1770280593811218</v>
+        <v>20.69420441642657</v>
       </c>
       <c r="U11" t="n">
-        <v>0.03591395911627394</v>
+        <v>3.974994251618649</v>
       </c>
     </row>
     <row r="12">
@@ -1212,64 +1212,64 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.5438198426873661</v>
+        <v>73.24146606853961</v>
       </c>
       <c r="C12" t="n">
-        <v>0.2013106974107253</v>
+        <v>35.012482745424</v>
       </c>
       <c r="D12" t="n">
-        <v>0.1199422967424666</v>
+        <v>19.14500564717642</v>
       </c>
       <c r="E12" t="n">
-        <v>0.1073335559929054</v>
+        <v>17.31743132701527</v>
       </c>
       <c r="F12" t="n">
-        <v>0.3121623755544702</v>
+        <v>117.6479300738739</v>
       </c>
       <c r="G12" t="n">
-        <v>0.1566591624062391</v>
+        <v>39.78473003089972</v>
       </c>
       <c r="H12" t="n">
-        <v>0.1611511710801652</v>
+        <v>22.87438245754333</v>
       </c>
       <c r="I12" t="n">
-        <v>0.1942260742168652</v>
+        <v>28.64022165003827</v>
       </c>
       <c r="J12" t="n">
-        <v>0.1781536440331379</v>
+        <v>27.80414180236518</v>
       </c>
       <c r="K12" t="n">
-        <v>0.1110292504346903</v>
+        <v>12.16785725437241</v>
       </c>
       <c r="L12" t="n">
         <v>0</v>
       </c>
       <c r="M12" t="n">
-        <v>0.2789449465500182</v>
+        <v>31.41798802796574</v>
       </c>
       <c r="N12" t="n">
-        <v>0.07420457469650456</v>
+        <v>8.077324124207692</v>
       </c>
       <c r="O12" t="n">
-        <v>0.08454131223359185</v>
+        <v>10.9073403556465</v>
       </c>
       <c r="P12" t="n">
-        <v>0.08242556546030702</v>
+        <v>13.56894661287347</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.0695904998791676</v>
+        <v>8.84544503083562</v>
       </c>
       <c r="R12" t="n">
-        <v>0.01672265672830477</v>
+        <v>2.741980715668803</v>
       </c>
       <c r="S12" t="n">
-        <v>0.03156120859936862</v>
+        <v>4.516471886212259</v>
       </c>
       <c r="T12" t="n">
-        <v>0.07188517269039021</v>
+        <v>12.35063924385549</v>
       </c>
       <c r="U12" t="n">
-        <v>0.02185572361814141</v>
+        <v>8.560136261440803</v>
       </c>
     </row>
     <row r="13">
@@ -1279,64 +1279,64 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>3.922967561809019</v>
+        <v>515.6608006389828</v>
       </c>
       <c r="C13" t="n">
-        <v>1.474978535206565</v>
+        <v>258.9815891272129</v>
       </c>
       <c r="D13" t="n">
-        <v>1.082787059394819</v>
+        <v>274.5571331803888</v>
       </c>
       <c r="E13" t="n">
-        <v>1.075584263980863</v>
+        <v>345.8321373052493</v>
       </c>
       <c r="F13" t="n">
-        <v>1.22675696107325</v>
+        <v>120.6489700032122</v>
       </c>
       <c r="G13" t="n">
-        <v>0.8265860502035145</v>
+        <v>103.8732221004126</v>
       </c>
       <c r="H13" t="n">
-        <v>1.588590084643201</v>
+        <v>433.6251574482413</v>
       </c>
       <c r="I13" t="n">
-        <v>1.366377798739836</v>
+        <v>186.2181677820286</v>
       </c>
       <c r="J13" t="n">
-        <v>1.170812233809938</v>
+        <v>145.6673403629809</v>
       </c>
       <c r="K13" t="n">
-        <v>1.041523263089528</v>
+        <v>197.0772999840456</v>
       </c>
       <c r="L13" t="n">
-        <v>0.2789449465500182</v>
+        <v>31.41798802796574</v>
       </c>
       <c r="M13" t="n">
         <v>0</v>
       </c>
       <c r="N13" t="n">
-        <v>0.6563044759393065</v>
+        <v>108.5495956104498</v>
       </c>
       <c r="O13" t="n">
-        <v>0.9041136715940549</v>
+        <v>267.7251541302313</v>
       </c>
       <c r="P13" t="n">
-        <v>0.6019715313673282</v>
+        <v>99.34276736320888</v>
       </c>
       <c r="Q13" t="n">
-        <v>0.5619980234744739</v>
+        <v>89.08933609939366</v>
       </c>
       <c r="R13" t="n">
-        <v>0.114907957211392</v>
+        <v>16.54622947158166</v>
       </c>
       <c r="S13" t="n">
-        <v>0.2055380437980335</v>
+        <v>22.98850868751008</v>
       </c>
       <c r="T13" t="n">
-        <v>0.4671698327759364</v>
+        <v>62.4505663961521</v>
       </c>
       <c r="U13" t="n">
-        <v>0.08786235971706423</v>
+        <v>9.433941642038565</v>
       </c>
     </row>
     <row r="14">
@@ -1346,64 +1346,64 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.9458255215543545</v>
+        <v>97.0434555773428</v>
       </c>
       <c r="C14" t="n">
-        <v>0.3398728936307667</v>
+        <v>42.21780754175937</v>
       </c>
       <c r="D14" t="n">
-        <v>0.2358105937030529</v>
+        <v>37.42108833563172</v>
       </c>
       <c r="E14" t="n">
-        <v>0.2113039957247282</v>
+        <v>33.9928814565047</v>
       </c>
       <c r="F14" t="n">
-        <v>0.3170686428569893</v>
+        <v>28.30803808649734</v>
       </c>
       <c r="G14" t="n">
-        <v>0.2071947498413253</v>
+        <v>22.11523703683941</v>
       </c>
       <c r="H14" t="n">
-        <v>0.3208769405714093</v>
+        <v>46.54788929841322</v>
       </c>
       <c r="I14" t="n">
-        <v>0.3346350200303586</v>
+        <v>36.83037390456204</v>
       </c>
       <c r="J14" t="n">
-        <v>0.3054930133291014</v>
+        <v>35.2219920856481</v>
       </c>
       <c r="K14" t="n">
-        <v>0.4059094980144862</v>
+        <v>170.1240629777096</v>
       </c>
       <c r="L14" t="n">
-        <v>0.07420457469650456</v>
+        <v>8.077324124207692</v>
       </c>
       <c r="M14" t="n">
-        <v>0.6563044759393065</v>
+        <v>108.5495956104498</v>
       </c>
       <c r="N14" t="n">
         <v>0</v>
       </c>
       <c r="O14" t="n">
-        <v>0.2242291628535487</v>
+        <v>55.10845608073137</v>
       </c>
       <c r="P14" t="n">
-        <v>0.1585829105182656</v>
+        <v>24.76298798666404</v>
       </c>
       <c r="Q14" t="n">
-        <v>0.1532823527122753</v>
+        <v>24.79212958345902</v>
       </c>
       <c r="R14" t="n">
-        <v>0.03178162819809446</v>
+        <v>4.813221780162849</v>
       </c>
       <c r="S14" t="n">
-        <v>0.06186181785860733</v>
+        <v>8.74313941242478</v>
       </c>
       <c r="T14" t="n">
-        <v>0.1200065519645127</v>
+        <v>14.37046824364747</v>
       </c>
       <c r="U14" t="n">
-        <v>0.02419711734925166</v>
+        <v>2.70715868842924</v>
       </c>
     </row>
     <row r="15">
@@ -1413,64 +1413,64 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1.087597558904144</v>
+        <v>134.9474873993719</v>
       </c>
       <c r="C15" t="n">
-        <v>0.4065264346844761</v>
+        <v>66.52426997853188</v>
       </c>
       <c r="D15" t="n">
-        <v>0.2799740315382225</v>
+        <v>57.59628932726799</v>
       </c>
       <c r="E15" t="n">
-        <v>0.2700702552886041</v>
+        <v>66.10139166955875</v>
       </c>
       <c r="F15" t="n">
-        <v>0.3685296416461688</v>
+        <v>40.72819249184865</v>
       </c>
       <c r="G15" t="n">
-        <v>0.2474484073603518</v>
+        <v>34.67867633617257</v>
       </c>
       <c r="H15" t="n">
-        <v>0.4339113337923615</v>
+        <v>108.2458795829952</v>
       </c>
       <c r="I15" t="n">
-        <v>0.4249074442317431</v>
+        <v>70.14576502997072</v>
       </c>
       <c r="J15" t="n">
-        <v>0.336527149460932</v>
+        <v>42.74594548528522</v>
       </c>
       <c r="K15" t="n">
-        <v>0.3332656445419659</v>
+        <v>81.27188082777515</v>
       </c>
       <c r="L15" t="n">
-        <v>0.08454131223359185</v>
+        <v>10.9073403556465</v>
       </c>
       <c r="M15" t="n">
-        <v>0.9041136715940549</v>
+        <v>267.7251541302313</v>
       </c>
       <c r="N15" t="n">
-        <v>0.2242291628535487</v>
+        <v>55.10845608073137</v>
       </c>
       <c r="O15" t="n">
         <v>0</v>
       </c>
       <c r="P15" t="n">
-        <v>0.1715809431896543</v>
+        <v>28.38731649155696</v>
       </c>
       <c r="Q15" t="n">
-        <v>0.2026435916913906</v>
+        <v>53.66267784029781</v>
       </c>
       <c r="R15" t="n">
-        <v>0.03846193084476533</v>
+        <v>7.87121270603196</v>
       </c>
       <c r="S15" t="n">
-        <v>0.0628004115182427</v>
+        <v>8.188708509427709</v>
       </c>
       <c r="T15" t="n">
-        <v>0.1483559931559536</v>
+        <v>25.14205586302417</v>
       </c>
       <c r="U15" t="n">
-        <v>0.02706362690533863</v>
+        <v>3.447783344031048</v>
       </c>
     </row>
     <row r="16">
@@ -1480,64 +1480,64 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1.333036089377373</v>
+        <v>346.9043594620259</v>
       </c>
       <c r="C16" t="n">
-        <v>0.4093730667284161</v>
+        <v>91.69208996276853</v>
       </c>
       <c r="D16" t="n">
-        <v>0.2884292850508153</v>
+        <v>85.33341443088079</v>
       </c>
       <c r="E16" t="n">
-        <v>0.2234972351990707</v>
+        <v>48.88911038034519</v>
       </c>
       <c r="F16" t="n">
-        <v>0.3516959041426887</v>
+        <v>47.34025871597547</v>
       </c>
       <c r="G16" t="n">
-        <v>0.2230132641965453</v>
+        <v>33.61877907668124</v>
       </c>
       <c r="H16" t="n">
-        <v>0.3139062177154358</v>
+        <v>52.26246126117292</v>
       </c>
       <c r="I16" t="n">
-        <v>0.3246362246489543</v>
+        <v>40.2683498525008</v>
       </c>
       <c r="J16" t="n">
-        <v>0.5190083083319154</v>
+        <v>227.7328192760707</v>
       </c>
       <c r="K16" t="n">
-        <v>0.2495374644451636</v>
+        <v>43.76487725055504</v>
       </c>
       <c r="L16" t="n">
-        <v>0.08242556546030702</v>
+        <v>13.56894661287347</v>
       </c>
       <c r="M16" t="n">
-        <v>0.6019715313673282</v>
+        <v>99.34276736320888</v>
       </c>
       <c r="N16" t="n">
-        <v>0.1585829105182656</v>
+        <v>24.76298798666404</v>
       </c>
       <c r="O16" t="n">
-        <v>0.1715809431896543</v>
+        <v>28.38731649155696</v>
       </c>
       <c r="P16" t="n">
         <v>0</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.1269010157860695</v>
+        <v>16.39394229109994</v>
       </c>
       <c r="R16" t="n">
-        <v>0.02813779584310747</v>
+        <v>3.937634374534195</v>
       </c>
       <c r="S16" t="n">
-        <v>0.06933069636367144</v>
+        <v>15.10866647300663</v>
       </c>
       <c r="T16" t="n">
-        <v>0.1149423202632534</v>
+        <v>15.08770425834458</v>
       </c>
       <c r="U16" t="n">
-        <v>0.02591953641458346</v>
+        <v>4.053033450127584</v>
       </c>
     </row>
     <row r="17">
@@ -1547,64 +1547,64 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.8136410108990793</v>
+        <v>80.81337308968041</v>
       </c>
       <c r="C17" t="n">
-        <v>0.3080831854734076</v>
+        <v>41.50563265940433</v>
       </c>
       <c r="D17" t="n">
-        <v>0.2008518829345858</v>
+        <v>30.19710947158296</v>
       </c>
       <c r="E17" t="n">
-        <v>0.1938515518072781</v>
+        <v>34.71561414850142</v>
       </c>
       <c r="F17" t="n">
-        <v>0.3032074755595441</v>
+        <v>32.97758148196699</v>
       </c>
       <c r="G17" t="n">
-        <v>0.2050814867229246</v>
+        <v>28.7378668712236</v>
       </c>
       <c r="H17" t="n">
-        <v>0.3190318309550865</v>
+        <v>61.35373183100276</v>
       </c>
       <c r="I17" t="n">
-        <v>0.3756539200634958</v>
+        <v>71.34584298681415</v>
       </c>
       <c r="J17" t="n">
-        <v>0.25454816801986</v>
+        <v>26.50887789075907</v>
       </c>
       <c r="K17" t="n">
-        <v>0.2200571445989937</v>
+        <v>32.75546275286384</v>
       </c>
       <c r="L17" t="n">
-        <v>0.0695904998791676</v>
+        <v>8.84544503083562</v>
       </c>
       <c r="M17" t="n">
-        <v>0.5619980234744739</v>
+        <v>89.08933609939366</v>
       </c>
       <c r="N17" t="n">
-        <v>0.1532823527122753</v>
+        <v>24.79212958345902</v>
       </c>
       <c r="O17" t="n">
-        <v>0.2026435916913906</v>
+        <v>53.66267784029781</v>
       </c>
       <c r="P17" t="n">
-        <v>0.1269010157860695</v>
+        <v>16.39394229109994</v>
       </c>
       <c r="Q17" t="n">
         <v>0</v>
       </c>
       <c r="R17" t="n">
-        <v>0.04004273501477658</v>
+        <v>13.44636956565316</v>
       </c>
       <c r="S17" t="n">
-        <v>0.04834940095670518</v>
+        <v>5.371151456393974</v>
       </c>
       <c r="T17" t="n">
-        <v>0.1371869396823843</v>
+        <v>29.48921123151991</v>
       </c>
       <c r="U17" t="n">
-        <v>0.022499555262292</v>
+        <v>2.885371258267296</v>
       </c>
     </row>
     <row r="18">
@@ -1614,64 +1614,64 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.180914330084948</v>
+        <v>19.58346306481534</v>
       </c>
       <c r="C18" t="n">
-        <v>0.06847852484732431</v>
+        <v>10.04675171482197</v>
       </c>
       <c r="D18" t="n">
-        <v>0.04353084885517617</v>
+        <v>6.746902998405186</v>
       </c>
       <c r="E18" t="n">
-        <v>0.04133862966660069</v>
+        <v>7.368040317792743</v>
       </c>
       <c r="F18" t="n">
-        <v>0.07238586604615192</v>
+        <v>10.01269413604668</v>
       </c>
       <c r="G18" t="n">
-        <v>0.04863836399039231</v>
+        <v>8.544977673146949</v>
       </c>
       <c r="H18" t="n">
-        <v>0.06661587561197994</v>
+        <v>12.18057984799809</v>
       </c>
       <c r="I18" t="n">
-        <v>0.08695661177093397</v>
+        <v>19.6426930247282</v>
       </c>
       <c r="J18" t="n">
-        <v>0.05720500012878239</v>
+        <v>6.644521418341258</v>
       </c>
       <c r="K18" t="n">
-        <v>0.04586044398245579</v>
+        <v>6.463137570691012</v>
       </c>
       <c r="L18" t="n">
-        <v>0.01672265672830477</v>
+        <v>2.741980715668803</v>
       </c>
       <c r="M18" t="n">
-        <v>0.114907957211392</v>
+        <v>16.54622947158166</v>
       </c>
       <c r="N18" t="n">
-        <v>0.03178162819809446</v>
+        <v>4.813221780162849</v>
       </c>
       <c r="O18" t="n">
-        <v>0.03846193084476533</v>
+        <v>7.87121270603196</v>
       </c>
       <c r="P18" t="n">
-        <v>0.02813779584310747</v>
+        <v>3.937634374534195</v>
       </c>
       <c r="Q18" t="n">
-        <v>0.04004273501477658</v>
+        <v>13.44636956565316</v>
       </c>
       <c r="R18" t="n">
         <v>0</v>
       </c>
       <c r="S18" t="n">
-        <v>0.01095420571207947</v>
+        <v>1.381410950996212</v>
       </c>
       <c r="T18" t="n">
-        <v>0.03504813001529814</v>
+        <v>11.10115034034277</v>
       </c>
       <c r="U18" t="n">
-        <v>0.005479485117406105</v>
+        <v>0.9332032886137153</v>
       </c>
     </row>
     <row r="19">
@@ -1681,64 +1681,64 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.3810106783015563</v>
+        <v>45.67233265707532</v>
       </c>
       <c r="C19" t="n">
-        <v>0.1304450846752479</v>
+        <v>17.04225531138226</v>
       </c>
       <c r="D19" t="n">
-        <v>0.08674531588967811</v>
+        <v>13.20371190782591</v>
       </c>
       <c r="E19" t="n">
-        <v>0.07378240204932295</v>
+        <v>10.16635119976261</v>
       </c>
       <c r="F19" t="n">
-        <v>0.1296521049734978</v>
+        <v>13.97056726190151</v>
       </c>
       <c r="G19" t="n">
-        <v>0.08064961509683467</v>
+        <v>9.334913483324714</v>
       </c>
       <c r="H19" t="n">
-        <v>0.108640028769557</v>
+        <v>12.62393291365497</v>
       </c>
       <c r="I19" t="n">
-        <v>0.118832145734371</v>
+        <v>11.61964733545398</v>
       </c>
       <c r="J19" t="n">
-        <v>0.1374899798657545</v>
+        <v>23.56154612713247</v>
       </c>
       <c r="K19" t="n">
-        <v>0.09309003696221417</v>
+        <v>13.41097756165878</v>
       </c>
       <c r="L19" t="n">
-        <v>0.03156120859936862</v>
+        <v>4.516471886212259</v>
       </c>
       <c r="M19" t="n">
-        <v>0.2055380437980335</v>
+        <v>22.98850868751008</v>
       </c>
       <c r="N19" t="n">
-        <v>0.06186181785860733</v>
+        <v>8.74313941242478</v>
       </c>
       <c r="O19" t="n">
-        <v>0.0628004115182427</v>
+        <v>8.188708509427709</v>
       </c>
       <c r="P19" t="n">
-        <v>0.06933069636367144</v>
+        <v>15.10866647300663</v>
       </c>
       <c r="Q19" t="n">
-        <v>0.04834940095670518</v>
+        <v>5.371151456393974</v>
       </c>
       <c r="R19" t="n">
-        <v>0.01095420571207947</v>
+        <v>1.381410950996212</v>
       </c>
       <c r="S19" t="n">
         <v>0</v>
       </c>
       <c r="T19" t="n">
-        <v>0.04316447745413925</v>
+        <v>4.721606764285506</v>
       </c>
       <c r="U19" t="n">
-        <v>0.01054545633187522</v>
+        <v>1.635307985792956</v>
       </c>
     </row>
     <row r="20">
@@ -1748,64 +1748,64 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.7633374454492508</v>
+        <v>83.14824786265031</v>
       </c>
       <c r="C20" t="n">
-        <v>0.2971229088388304</v>
+        <v>46.61109119060586</v>
       </c>
       <c r="D20" t="n">
-        <v>0.1823572814217435</v>
+        <v>28.00138615746715</v>
       </c>
       <c r="E20" t="n">
-        <v>0.1765718719894737</v>
+        <v>32.52336967366866</v>
       </c>
       <c r="F20" t="n">
-        <v>0.3231051337461743</v>
+        <v>50.82230770753425</v>
       </c>
       <c r="G20" t="n">
-        <v>0.229856606740604</v>
+        <v>51.98011656689501</v>
       </c>
       <c r="H20" t="n">
-        <v>0.2878116514519349</v>
+        <v>55.75196439482628</v>
       </c>
       <c r="I20" t="n">
-        <v>0.4753837331846074</v>
+        <v>189.6654677537916</v>
       </c>
       <c r="J20" t="n">
-        <v>0.2366168888707608</v>
+        <v>26.48796839735648</v>
       </c>
       <c r="K20" t="n">
-        <v>0.1770280593811218</v>
+        <v>20.69420441642657</v>
       </c>
       <c r="L20" t="n">
-        <v>0.07188517269039021</v>
+        <v>12.35063924385549</v>
       </c>
       <c r="M20" t="n">
-        <v>0.4671698327759364</v>
+        <v>62.4505663961521</v>
       </c>
       <c r="N20" t="n">
-        <v>0.1200065519645127</v>
+        <v>14.37046824364747</v>
       </c>
       <c r="O20" t="n">
-        <v>0.1483559931559536</v>
+        <v>25.14205586302417</v>
       </c>
       <c r="P20" t="n">
-        <v>0.1149423202632534</v>
+        <v>15.08770425834458</v>
       </c>
       <c r="Q20" t="n">
-        <v>0.1371869396823843</v>
+        <v>29.48921123151991</v>
       </c>
       <c r="R20" t="n">
-        <v>0.03504813001529814</v>
+        <v>11.10115034034277</v>
       </c>
       <c r="S20" t="n">
-        <v>0.04316447745413925</v>
+        <v>4.721606764285506</v>
       </c>
       <c r="T20" t="n">
         <v>0</v>
       </c>
       <c r="U20" t="n">
-        <v>0.02260275175881474</v>
+        <v>3.687959577928079</v>
       </c>
     </row>
     <row r="21">
@@ -1815,61 +1815,61 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.1650575341562291</v>
+        <v>19.55206696407565</v>
       </c>
       <c r="C21" t="n">
-        <v>0.06024339699417602</v>
+        <v>8.936981748599937</v>
       </c>
       <c r="D21" t="n">
-        <v>0.03699143648735424</v>
+        <v>5.376883589600534</v>
       </c>
       <c r="E21" t="n">
-        <v>0.03305904368634398</v>
+        <v>4.843259864789729</v>
       </c>
       <c r="F21" t="n">
-        <v>0.07756568373691207</v>
+        <v>16.65009348587779</v>
       </c>
       <c r="G21" t="n">
-        <v>0.04439523944085714</v>
+        <v>8.543440697881632</v>
       </c>
       <c r="H21" t="n">
-        <v>0.04994393323830284</v>
+        <v>6.524543999018621</v>
       </c>
       <c r="I21" t="n">
-        <v>0.06011014164273937</v>
+        <v>8.132898353418625</v>
       </c>
       <c r="J21" t="n">
-        <v>0.055134499732434</v>
+        <v>7.894816085537324</v>
       </c>
       <c r="K21" t="n">
-        <v>0.03591395911627394</v>
+        <v>3.974994251618649</v>
       </c>
       <c r="L21" t="n">
-        <v>0.02185572361814141</v>
+        <v>8.560136261440803</v>
       </c>
       <c r="M21" t="n">
-        <v>0.08786235971706423</v>
+        <v>9.433941642038565</v>
       </c>
       <c r="N21" t="n">
-        <v>0.02419711734925166</v>
+        <v>2.70715868842924</v>
       </c>
       <c r="O21" t="n">
-        <v>0.02706362690533863</v>
+        <v>3.447783344031048</v>
       </c>
       <c r="P21" t="n">
-        <v>0.02591953641458346</v>
+        <v>4.053033450127584</v>
       </c>
       <c r="Q21" t="n">
-        <v>0.022499555262292</v>
+        <v>2.885371258267296</v>
       </c>
       <c r="R21" t="n">
-        <v>0.005479485117406105</v>
+        <v>0.9332032886137153</v>
       </c>
       <c r="S21" t="n">
-        <v>0.01054545633187522</v>
+        <v>1.635307985792956</v>
       </c>
       <c r="T21" t="n">
-        <v>0.02260275175881474</v>
+        <v>3.687959577928079</v>
       </c>
       <c r="U21" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
added yield calculater, changed demand to integers, saved files for demand of 2026, all distances and all yields
</commit_message>
<xml_diff>
--- a/Code/Estimated Data/demand_2026_matrix.xlsx
+++ b/Code/Estimated Data/demand_2026_matrix.xlsx
@@ -545,61 +545,61 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>1045.501704723878</v>
+        <v>1045</v>
       </c>
       <c r="D2" t="n">
-        <v>681.5869269208697</v>
+        <v>681</v>
       </c>
       <c r="E2" t="n">
-        <v>338.9306982050842</v>
+        <v>338</v>
       </c>
       <c r="F2" t="n">
-        <v>284.4217910886661</v>
+        <v>284</v>
       </c>
       <c r="G2" t="n">
-        <v>214.5323724753912</v>
+        <v>214</v>
       </c>
       <c r="H2" t="n">
-        <v>321.7211544727224</v>
+        <v>321</v>
       </c>
       <c r="I2" t="n">
-        <v>234.0632048431902</v>
+        <v>234</v>
       </c>
       <c r="J2" t="n">
-        <v>708.6677278466523</v>
+        <v>708</v>
       </c>
       <c r="K2" t="n">
-        <v>166.1826814839588</v>
+        <v>166</v>
       </c>
       <c r="L2" t="n">
-        <v>73.24146606853961</v>
+        <v>73</v>
       </c>
       <c r="M2" t="n">
-        <v>515.6608006389828</v>
+        <v>515</v>
       </c>
       <c r="N2" t="n">
-        <v>97.0434555773428</v>
+        <v>97</v>
       </c>
       <c r="O2" t="n">
-        <v>134.9474873993719</v>
+        <v>134</v>
       </c>
       <c r="P2" t="n">
-        <v>346.9043594620259</v>
+        <v>346</v>
       </c>
       <c r="Q2" t="n">
-        <v>80.81337308968041</v>
+        <v>80</v>
       </c>
       <c r="R2" t="n">
-        <v>19.58346306481534</v>
+        <v>19</v>
       </c>
       <c r="S2" t="n">
-        <v>45.67233265707532</v>
+        <v>45</v>
       </c>
       <c r="T2" t="n">
-        <v>83.14824786265031</v>
+        <v>83</v>
       </c>
       <c r="U2" t="n">
-        <v>19.55206696407565</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3">
@@ -609,64 +609,64 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1045.501704723878</v>
+        <v>1045</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>281.8681414562378</v>
+        <v>281</v>
       </c>
       <c r="E3" t="n">
-        <v>227.6403930034599</v>
+        <v>227</v>
       </c>
       <c r="F3" t="n">
-        <v>150.7028303599278</v>
+        <v>150</v>
       </c>
       <c r="G3" t="n">
-        <v>131.1590154118439</v>
+        <v>131</v>
       </c>
       <c r="H3" t="n">
-        <v>203.8393959382139</v>
+        <v>203</v>
       </c>
       <c r="I3" t="n">
-        <v>140.2477869647435</v>
+        <v>140</v>
       </c>
       <c r="J3" t="n">
-        <v>173.5791897611845</v>
+        <v>173</v>
       </c>
       <c r="K3" t="n">
-        <v>70.32530360250405</v>
+        <v>70</v>
       </c>
       <c r="L3" t="n">
-        <v>35.012482745424</v>
+        <v>35</v>
       </c>
       <c r="M3" t="n">
-        <v>258.9815891272129</v>
+        <v>258</v>
       </c>
       <c r="N3" t="n">
-        <v>42.21780754175937</v>
+        <v>42</v>
       </c>
       <c r="O3" t="n">
-        <v>66.52426997853188</v>
+        <v>66</v>
       </c>
       <c r="P3" t="n">
-        <v>91.69208996276853</v>
+        <v>91</v>
       </c>
       <c r="Q3" t="n">
-        <v>41.50563265940433</v>
+        <v>41</v>
       </c>
       <c r="R3" t="n">
-        <v>10.04675171482197</v>
+        <v>10</v>
       </c>
       <c r="S3" t="n">
-        <v>17.04225531138226</v>
+        <v>17</v>
       </c>
       <c r="T3" t="n">
-        <v>46.61109119060586</v>
+        <v>46</v>
       </c>
       <c r="U3" t="n">
-        <v>8.936981748599937</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">
@@ -676,64 +676,64 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>681.5869269208697</v>
+        <v>681</v>
       </c>
       <c r="C4" t="n">
-        <v>281.8681414562378</v>
+        <v>281</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>198.0844625790089</v>
+        <v>198</v>
       </c>
       <c r="F4" t="n">
-        <v>74.90964325441705</v>
+        <v>74</v>
       </c>
       <c r="G4" t="n">
-        <v>61.6425790025206</v>
+        <v>61</v>
       </c>
       <c r="H4" t="n">
-        <v>146.555946650177</v>
+        <v>146</v>
       </c>
       <c r="I4" t="n">
-        <v>82.16593044605925</v>
+        <v>82</v>
       </c>
       <c r="J4" t="n">
-        <v>127.4504865588624</v>
+        <v>127</v>
       </c>
       <c r="K4" t="n">
-        <v>67.19736812210172</v>
+        <v>67</v>
       </c>
       <c r="L4" t="n">
-        <v>19.14500564717642</v>
+        <v>19</v>
       </c>
       <c r="M4" t="n">
-        <v>274.5571331803888</v>
+        <v>274</v>
       </c>
       <c r="N4" t="n">
-        <v>37.42108833563172</v>
+        <v>37</v>
       </c>
       <c r="O4" t="n">
-        <v>57.59628932726799</v>
+        <v>57</v>
       </c>
       <c r="P4" t="n">
-        <v>85.33341443088079</v>
+        <v>85</v>
       </c>
       <c r="Q4" t="n">
-        <v>30.19710947158296</v>
+        <v>30</v>
       </c>
       <c r="R4" t="n">
-        <v>6.746902998405186</v>
+        <v>6</v>
       </c>
       <c r="S4" t="n">
-        <v>13.20371190782591</v>
+        <v>13</v>
       </c>
       <c r="T4" t="n">
-        <v>28.00138615746715</v>
+        <v>28</v>
       </c>
       <c r="U4" t="n">
-        <v>5.376883589600534</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">
@@ -743,64 +743,64 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>338.9306982050842</v>
+        <v>338</v>
       </c>
       <c r="C5" t="n">
-        <v>227.6403930034599</v>
+        <v>227</v>
       </c>
       <c r="D5" t="n">
-        <v>198.0844625790089</v>
+        <v>198</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>70.86788499495998</v>
+        <v>70</v>
       </c>
       <c r="G5" t="n">
-        <v>64.94077468183021</v>
+        <v>64</v>
       </c>
       <c r="H5" t="n">
-        <v>318.4723755706087</v>
+        <v>318</v>
       </c>
       <c r="I5" t="n">
-        <v>104.6726220019602</v>
+        <v>104</v>
       </c>
       <c r="J5" t="n">
-        <v>78.52939523939308</v>
+        <v>78</v>
       </c>
       <c r="K5" t="n">
-        <v>57.91326073029241</v>
+        <v>57</v>
       </c>
       <c r="L5" t="n">
-        <v>17.31743132701527</v>
+        <v>17</v>
       </c>
       <c r="M5" t="n">
-        <v>345.8321373052493</v>
+        <v>345</v>
       </c>
       <c r="N5" t="n">
-        <v>33.9928814565047</v>
+        <v>33</v>
       </c>
       <c r="O5" t="n">
-        <v>66.10139166955875</v>
+        <v>66</v>
       </c>
       <c r="P5" t="n">
-        <v>48.88911038034519</v>
+        <v>48</v>
       </c>
       <c r="Q5" t="n">
-        <v>34.71561414850142</v>
+        <v>34</v>
       </c>
       <c r="R5" t="n">
-        <v>7.368040317792743</v>
+        <v>7</v>
       </c>
       <c r="S5" t="n">
-        <v>10.16635119976261</v>
+        <v>10</v>
       </c>
       <c r="T5" t="n">
-        <v>32.52336967366866</v>
+        <v>32</v>
       </c>
       <c r="U5" t="n">
-        <v>4.843259864789729</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
@@ -810,64 +810,64 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>284.4217910886661</v>
+        <v>284</v>
       </c>
       <c r="C6" t="n">
-        <v>150.7028303599278</v>
+        <v>150</v>
       </c>
       <c r="D6" t="n">
-        <v>74.90964325441705</v>
+        <v>74</v>
       </c>
       <c r="E6" t="n">
-        <v>70.86788499495998</v>
+        <v>70</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>263.3734819180988</v>
+        <v>263</v>
       </c>
       <c r="H6" t="n">
-        <v>94.17366998159903</v>
+        <v>94</v>
       </c>
       <c r="I6" t="n">
-        <v>123.4698193430533</v>
+        <v>123</v>
       </c>
       <c r="J6" t="n">
-        <v>96.35336660463844</v>
+        <v>96</v>
       </c>
       <c r="K6" t="n">
-        <v>43.09960859506008</v>
+        <v>43</v>
       </c>
       <c r="L6" t="n">
-        <v>117.6479300738739</v>
+        <v>117</v>
       </c>
       <c r="M6" t="n">
-        <v>120.6489700032122</v>
+        <v>120</v>
       </c>
       <c r="N6" t="n">
-        <v>28.30803808649734</v>
+        <v>28</v>
       </c>
       <c r="O6" t="n">
-        <v>40.72819249184865</v>
+        <v>40</v>
       </c>
       <c r="P6" t="n">
-        <v>47.34025871597547</v>
+        <v>47</v>
       </c>
       <c r="Q6" t="n">
-        <v>32.97758148196699</v>
+        <v>32</v>
       </c>
       <c r="R6" t="n">
-        <v>10.01269413604668</v>
+        <v>10</v>
       </c>
       <c r="S6" t="n">
-        <v>13.97056726190151</v>
+        <v>13</v>
       </c>
       <c r="T6" t="n">
-        <v>50.82230770753425</v>
+        <v>50</v>
       </c>
       <c r="U6" t="n">
-        <v>16.65009348587779</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7">
@@ -877,64 +877,64 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>214.5323724753912</v>
+        <v>214</v>
       </c>
       <c r="C7" t="n">
-        <v>131.1590154118439</v>
+        <v>131</v>
       </c>
       <c r="D7" t="n">
-        <v>61.6425790025206</v>
+        <v>61</v>
       </c>
       <c r="E7" t="n">
-        <v>64.94077468183021</v>
+        <v>64</v>
       </c>
       <c r="F7" t="n">
-        <v>263.3734819180988</v>
+        <v>263</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>91.11941768350989</v>
+        <v>91</v>
       </c>
       <c r="I7" t="n">
-        <v>138.6482841535388</v>
+        <v>138</v>
       </c>
       <c r="J7" t="n">
-        <v>65.02077305932224</v>
+        <v>65</v>
       </c>
       <c r="K7" t="n">
-        <v>33.74232519574387</v>
+        <v>33</v>
       </c>
       <c r="L7" t="n">
-        <v>39.78473003089972</v>
+        <v>39</v>
       </c>
       <c r="M7" t="n">
-        <v>103.8732221004126</v>
+        <v>103</v>
       </c>
       <c r="N7" t="n">
-        <v>22.11523703683941</v>
+        <v>22</v>
       </c>
       <c r="O7" t="n">
-        <v>34.67867633617257</v>
+        <v>34</v>
       </c>
       <c r="P7" t="n">
-        <v>33.61877907668124</v>
+        <v>33</v>
       </c>
       <c r="Q7" t="n">
-        <v>28.7378668712236</v>
+        <v>28</v>
       </c>
       <c r="R7" t="n">
-        <v>8.544977673146949</v>
+        <v>8</v>
       </c>
       <c r="S7" t="n">
-        <v>9.334913483324714</v>
+        <v>9</v>
       </c>
       <c r="T7" t="n">
-        <v>51.98011656689501</v>
+        <v>51</v>
       </c>
       <c r="U7" t="n">
-        <v>8.543440697881632</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8">
@@ -944,64 +944,64 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>321.7211544727224</v>
+        <v>321</v>
       </c>
       <c r="C8" t="n">
-        <v>203.8393959382139</v>
+        <v>203</v>
       </c>
       <c r="D8" t="n">
-        <v>146.555946650177</v>
+        <v>146</v>
       </c>
       <c r="E8" t="n">
-        <v>318.4723755706087</v>
+        <v>318</v>
       </c>
       <c r="F8" t="n">
-        <v>94.17366998159903</v>
+        <v>94</v>
       </c>
       <c r="G8" t="n">
-        <v>91.11941768350989</v>
+        <v>91</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>197.2448578266715</v>
+        <v>197</v>
       </c>
       <c r="J8" t="n">
-        <v>85.17096310026463</v>
+        <v>85</v>
       </c>
       <c r="K8" t="n">
-        <v>75.07698709470658</v>
+        <v>75</v>
       </c>
       <c r="L8" t="n">
-        <v>22.87438245754333</v>
+        <v>22</v>
       </c>
       <c r="M8" t="n">
-        <v>433.6251574482413</v>
+        <v>433</v>
       </c>
       <c r="N8" t="n">
-        <v>46.54788929841322</v>
+        <v>46</v>
       </c>
       <c r="O8" t="n">
-        <v>108.2458795829952</v>
+        <v>108</v>
       </c>
       <c r="P8" t="n">
-        <v>52.26246126117292</v>
+        <v>52</v>
       </c>
       <c r="Q8" t="n">
-        <v>61.35373183100276</v>
+        <v>61</v>
       </c>
       <c r="R8" t="n">
-        <v>12.18057984799809</v>
+        <v>12</v>
       </c>
       <c r="S8" t="n">
-        <v>12.62393291365497</v>
+        <v>12</v>
       </c>
       <c r="T8" t="n">
-        <v>55.75196439482628</v>
+        <v>55</v>
       </c>
       <c r="U8" t="n">
-        <v>6.524543999018621</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9">
@@ -1011,64 +1011,64 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>234.0632048431902</v>
+        <v>234</v>
       </c>
       <c r="C9" t="n">
-        <v>140.2477869647435</v>
+        <v>140</v>
       </c>
       <c r="D9" t="n">
-        <v>82.16593044605925</v>
+        <v>82</v>
       </c>
       <c r="E9" t="n">
-        <v>104.6726220019602</v>
+        <v>104</v>
       </c>
       <c r="F9" t="n">
-        <v>123.4698193430533</v>
+        <v>123</v>
       </c>
       <c r="G9" t="n">
-        <v>138.6482841535388</v>
+        <v>138</v>
       </c>
       <c r="H9" t="n">
-        <v>197.2448578266715</v>
+        <v>197</v>
       </c>
       <c r="I9" t="n">
         <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>70.24707606986435</v>
+        <v>70</v>
       </c>
       <c r="K9" t="n">
-        <v>54.53299256456867</v>
+        <v>54</v>
       </c>
       <c r="L9" t="n">
-        <v>28.64022165003827</v>
+        <v>28</v>
       </c>
       <c r="M9" t="n">
-        <v>186.2181677820286</v>
+        <v>186</v>
       </c>
       <c r="N9" t="n">
-        <v>36.83037390456204</v>
+        <v>36</v>
       </c>
       <c r="O9" t="n">
-        <v>70.14576502997072</v>
+        <v>70</v>
       </c>
       <c r="P9" t="n">
-        <v>40.2683498525008</v>
+        <v>40</v>
       </c>
       <c r="Q9" t="n">
-        <v>71.34584298681415</v>
+        <v>71</v>
       </c>
       <c r="R9" t="n">
-        <v>19.6426930247282</v>
+        <v>19</v>
       </c>
       <c r="S9" t="n">
-        <v>11.61964733545398</v>
+        <v>11</v>
       </c>
       <c r="T9" t="n">
-        <v>189.6654677537916</v>
+        <v>189</v>
       </c>
       <c r="U9" t="n">
-        <v>8.132898353418625</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
@@ -1078,64 +1078,64 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>708.6677278466523</v>
+        <v>708</v>
       </c>
       <c r="C10" t="n">
-        <v>173.5791897611845</v>
+        <v>173</v>
       </c>
       <c r="D10" t="n">
-        <v>127.4504865588624</v>
+        <v>127</v>
       </c>
       <c r="E10" t="n">
-        <v>78.52939523939308</v>
+        <v>78</v>
       </c>
       <c r="F10" t="n">
-        <v>96.35336660463844</v>
+        <v>96</v>
       </c>
       <c r="G10" t="n">
-        <v>65.02077305932224</v>
+        <v>65</v>
       </c>
       <c r="H10" t="n">
-        <v>85.17096310026463</v>
+        <v>85</v>
       </c>
       <c r="I10" t="n">
-        <v>70.24707606986435</v>
+        <v>70</v>
       </c>
       <c r="J10" t="n">
         <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>59.37777136911156</v>
+        <v>59</v>
       </c>
       <c r="L10" t="n">
-        <v>27.80414180236518</v>
+        <v>27</v>
       </c>
       <c r="M10" t="n">
-        <v>145.6673403629809</v>
+        <v>145</v>
       </c>
       <c r="N10" t="n">
-        <v>35.2219920856481</v>
+        <v>35</v>
       </c>
       <c r="O10" t="n">
-        <v>42.74594548528522</v>
+        <v>42</v>
       </c>
       <c r="P10" t="n">
-        <v>227.7328192760707</v>
+        <v>227</v>
       </c>
       <c r="Q10" t="n">
-        <v>26.50887789075907</v>
+        <v>26</v>
       </c>
       <c r="R10" t="n">
-        <v>6.644521418341258</v>
+        <v>6</v>
       </c>
       <c r="S10" t="n">
-        <v>23.56154612713247</v>
+        <v>23</v>
       </c>
       <c r="T10" t="n">
-        <v>26.48796839735648</v>
+        <v>26</v>
       </c>
       <c r="U10" t="n">
-        <v>7.894816085537324</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11">
@@ -1145,64 +1145,64 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>166.1826814839588</v>
+        <v>166</v>
       </c>
       <c r="C11" t="n">
-        <v>70.32530360250405</v>
+        <v>70</v>
       </c>
       <c r="D11" t="n">
-        <v>67.19736812210172</v>
+        <v>67</v>
       </c>
       <c r="E11" t="n">
-        <v>57.91326073029241</v>
+        <v>57</v>
       </c>
       <c r="F11" t="n">
-        <v>43.09960859506008</v>
+        <v>43</v>
       </c>
       <c r="G11" t="n">
-        <v>33.74232519574387</v>
+        <v>33</v>
       </c>
       <c r="H11" t="n">
-        <v>75.07698709470658</v>
+        <v>75</v>
       </c>
       <c r="I11" t="n">
-        <v>54.53299256456867</v>
+        <v>54</v>
       </c>
       <c r="J11" t="n">
-        <v>59.37777136911156</v>
+        <v>59</v>
       </c>
       <c r="K11" t="n">
         <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>12.16785725437241</v>
+        <v>12</v>
       </c>
       <c r="M11" t="n">
-        <v>197.0772999840456</v>
+        <v>197</v>
       </c>
       <c r="N11" t="n">
-        <v>170.1240629777096</v>
+        <v>170</v>
       </c>
       <c r="O11" t="n">
-        <v>81.27188082777515</v>
+        <v>81</v>
       </c>
       <c r="P11" t="n">
-        <v>43.76487725055504</v>
+        <v>43</v>
       </c>
       <c r="Q11" t="n">
-        <v>32.75546275286384</v>
+        <v>32</v>
       </c>
       <c r="R11" t="n">
-        <v>6.463137570691012</v>
+        <v>6</v>
       </c>
       <c r="S11" t="n">
-        <v>13.41097756165878</v>
+        <v>13</v>
       </c>
       <c r="T11" t="n">
-        <v>20.69420441642657</v>
+        <v>20</v>
       </c>
       <c r="U11" t="n">
-        <v>3.974994251618649</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12">
@@ -1212,64 +1212,64 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>73.24146606853961</v>
+        <v>73</v>
       </c>
       <c r="C12" t="n">
-        <v>35.012482745424</v>
+        <v>35</v>
       </c>
       <c r="D12" t="n">
-        <v>19.14500564717642</v>
+        <v>19</v>
       </c>
       <c r="E12" t="n">
-        <v>17.31743132701527</v>
+        <v>17</v>
       </c>
       <c r="F12" t="n">
-        <v>117.6479300738739</v>
+        <v>117</v>
       </c>
       <c r="G12" t="n">
-        <v>39.78473003089972</v>
+        <v>39</v>
       </c>
       <c r="H12" t="n">
-        <v>22.87438245754333</v>
+        <v>22</v>
       </c>
       <c r="I12" t="n">
-        <v>28.64022165003827</v>
+        <v>28</v>
       </c>
       <c r="J12" t="n">
-        <v>27.80414180236518</v>
+        <v>27</v>
       </c>
       <c r="K12" t="n">
-        <v>12.16785725437241</v>
+        <v>12</v>
       </c>
       <c r="L12" t="n">
         <v>0</v>
       </c>
       <c r="M12" t="n">
-        <v>31.41798802796574</v>
+        <v>31</v>
       </c>
       <c r="N12" t="n">
-        <v>8.077324124207692</v>
+        <v>8</v>
       </c>
       <c r="O12" t="n">
-        <v>10.9073403556465</v>
+        <v>10</v>
       </c>
       <c r="P12" t="n">
-        <v>13.56894661287347</v>
+        <v>13</v>
       </c>
       <c r="Q12" t="n">
-        <v>8.84544503083562</v>
+        <v>8</v>
       </c>
       <c r="R12" t="n">
-        <v>2.741980715668803</v>
+        <v>2</v>
       </c>
       <c r="S12" t="n">
-        <v>4.516471886212259</v>
+        <v>4</v>
       </c>
       <c r="T12" t="n">
-        <v>12.35063924385549</v>
+        <v>12</v>
       </c>
       <c r="U12" t="n">
-        <v>8.560136261440803</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13">
@@ -1279,64 +1279,64 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>515.6608006389828</v>
+        <v>515</v>
       </c>
       <c r="C13" t="n">
-        <v>258.9815891272129</v>
+        <v>258</v>
       </c>
       <c r="D13" t="n">
-        <v>274.5571331803888</v>
+        <v>274</v>
       </c>
       <c r="E13" t="n">
-        <v>345.8321373052493</v>
+        <v>345</v>
       </c>
       <c r="F13" t="n">
-        <v>120.6489700032122</v>
+        <v>120</v>
       </c>
       <c r="G13" t="n">
-        <v>103.8732221004126</v>
+        <v>103</v>
       </c>
       <c r="H13" t="n">
-        <v>433.6251574482413</v>
+        <v>433</v>
       </c>
       <c r="I13" t="n">
-        <v>186.2181677820286</v>
+        <v>186</v>
       </c>
       <c r="J13" t="n">
-        <v>145.6673403629809</v>
+        <v>145</v>
       </c>
       <c r="K13" t="n">
-        <v>197.0772999840456</v>
+        <v>197</v>
       </c>
       <c r="L13" t="n">
-        <v>31.41798802796574</v>
+        <v>31</v>
       </c>
       <c r="M13" t="n">
         <v>0</v>
       </c>
       <c r="N13" t="n">
-        <v>108.5495956104498</v>
+        <v>108</v>
       </c>
       <c r="O13" t="n">
-        <v>267.7251541302313</v>
+        <v>267</v>
       </c>
       <c r="P13" t="n">
-        <v>99.34276736320888</v>
+        <v>99</v>
       </c>
       <c r="Q13" t="n">
-        <v>89.08933609939366</v>
+        <v>89</v>
       </c>
       <c r="R13" t="n">
-        <v>16.54622947158166</v>
+        <v>16</v>
       </c>
       <c r="S13" t="n">
-        <v>22.98850868751008</v>
+        <v>22</v>
       </c>
       <c r="T13" t="n">
-        <v>62.4505663961521</v>
+        <v>62</v>
       </c>
       <c r="U13" t="n">
-        <v>9.433941642038565</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14">
@@ -1346,64 +1346,64 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>97.0434555773428</v>
+        <v>97</v>
       </c>
       <c r="C14" t="n">
-        <v>42.21780754175937</v>
+        <v>42</v>
       </c>
       <c r="D14" t="n">
-        <v>37.42108833563172</v>
+        <v>37</v>
       </c>
       <c r="E14" t="n">
-        <v>33.9928814565047</v>
+        <v>33</v>
       </c>
       <c r="F14" t="n">
-        <v>28.30803808649734</v>
+        <v>28</v>
       </c>
       <c r="G14" t="n">
-        <v>22.11523703683941</v>
+        <v>22</v>
       </c>
       <c r="H14" t="n">
-        <v>46.54788929841322</v>
+        <v>46</v>
       </c>
       <c r="I14" t="n">
-        <v>36.83037390456204</v>
+        <v>36</v>
       </c>
       <c r="J14" t="n">
-        <v>35.2219920856481</v>
+        <v>35</v>
       </c>
       <c r="K14" t="n">
-        <v>170.1240629777096</v>
+        <v>170</v>
       </c>
       <c r="L14" t="n">
-        <v>8.077324124207692</v>
+        <v>8</v>
       </c>
       <c r="M14" t="n">
-        <v>108.5495956104498</v>
+        <v>108</v>
       </c>
       <c r="N14" t="n">
         <v>0</v>
       </c>
       <c r="O14" t="n">
-        <v>55.10845608073137</v>
+        <v>55</v>
       </c>
       <c r="P14" t="n">
-        <v>24.76298798666404</v>
+        <v>24</v>
       </c>
       <c r="Q14" t="n">
-        <v>24.79212958345902</v>
+        <v>24</v>
       </c>
       <c r="R14" t="n">
-        <v>4.813221780162849</v>
+        <v>4</v>
       </c>
       <c r="S14" t="n">
-        <v>8.74313941242478</v>
+        <v>8</v>
       </c>
       <c r="T14" t="n">
-        <v>14.37046824364747</v>
+        <v>14</v>
       </c>
       <c r="U14" t="n">
-        <v>2.70715868842924</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15">
@@ -1413,64 +1413,64 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>134.9474873993719</v>
+        <v>134</v>
       </c>
       <c r="C15" t="n">
-        <v>66.52426997853188</v>
+        <v>66</v>
       </c>
       <c r="D15" t="n">
-        <v>57.59628932726799</v>
+        <v>57</v>
       </c>
       <c r="E15" t="n">
-        <v>66.10139166955875</v>
+        <v>66</v>
       </c>
       <c r="F15" t="n">
-        <v>40.72819249184865</v>
+        <v>40</v>
       </c>
       <c r="G15" t="n">
-        <v>34.67867633617257</v>
+        <v>34</v>
       </c>
       <c r="H15" t="n">
-        <v>108.2458795829952</v>
+        <v>108</v>
       </c>
       <c r="I15" t="n">
-        <v>70.14576502997072</v>
+        <v>70</v>
       </c>
       <c r="J15" t="n">
-        <v>42.74594548528522</v>
+        <v>42</v>
       </c>
       <c r="K15" t="n">
-        <v>81.27188082777515</v>
+        <v>81</v>
       </c>
       <c r="L15" t="n">
-        <v>10.9073403556465</v>
+        <v>10</v>
       </c>
       <c r="M15" t="n">
-        <v>267.7251541302313</v>
+        <v>267</v>
       </c>
       <c r="N15" t="n">
-        <v>55.10845608073137</v>
+        <v>55</v>
       </c>
       <c r="O15" t="n">
         <v>0</v>
       </c>
       <c r="P15" t="n">
-        <v>28.38731649155696</v>
+        <v>28</v>
       </c>
       <c r="Q15" t="n">
-        <v>53.66267784029781</v>
+        <v>53</v>
       </c>
       <c r="R15" t="n">
-        <v>7.87121270603196</v>
+        <v>7</v>
       </c>
       <c r="S15" t="n">
-        <v>8.188708509427709</v>
+        <v>8</v>
       </c>
       <c r="T15" t="n">
-        <v>25.14205586302417</v>
+        <v>25</v>
       </c>
       <c r="U15" t="n">
-        <v>3.447783344031048</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16">
@@ -1480,64 +1480,64 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>346.9043594620259</v>
+        <v>346</v>
       </c>
       <c r="C16" t="n">
-        <v>91.69208996276853</v>
+        <v>91</v>
       </c>
       <c r="D16" t="n">
-        <v>85.33341443088079</v>
+        <v>85</v>
       </c>
       <c r="E16" t="n">
-        <v>48.88911038034519</v>
+        <v>48</v>
       </c>
       <c r="F16" t="n">
-        <v>47.34025871597547</v>
+        <v>47</v>
       </c>
       <c r="G16" t="n">
-        <v>33.61877907668124</v>
+        <v>33</v>
       </c>
       <c r="H16" t="n">
-        <v>52.26246126117292</v>
+        <v>52</v>
       </c>
       <c r="I16" t="n">
-        <v>40.2683498525008</v>
+        <v>40</v>
       </c>
       <c r="J16" t="n">
-        <v>227.7328192760707</v>
+        <v>227</v>
       </c>
       <c r="K16" t="n">
-        <v>43.76487725055504</v>
+        <v>43</v>
       </c>
       <c r="L16" t="n">
-        <v>13.56894661287347</v>
+        <v>13</v>
       </c>
       <c r="M16" t="n">
-        <v>99.34276736320888</v>
+        <v>99</v>
       </c>
       <c r="N16" t="n">
-        <v>24.76298798666404</v>
+        <v>24</v>
       </c>
       <c r="O16" t="n">
-        <v>28.38731649155696</v>
+        <v>28</v>
       </c>
       <c r="P16" t="n">
         <v>0</v>
       </c>
       <c r="Q16" t="n">
-        <v>16.39394229109994</v>
+        <v>16</v>
       </c>
       <c r="R16" t="n">
-        <v>3.937634374534195</v>
+        <v>3</v>
       </c>
       <c r="S16" t="n">
-        <v>15.10866647300663</v>
+        <v>15</v>
       </c>
       <c r="T16" t="n">
-        <v>15.08770425834458</v>
+        <v>15</v>
       </c>
       <c r="U16" t="n">
-        <v>4.053033450127584</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17">
@@ -1547,64 +1547,64 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>80.81337308968041</v>
+        <v>80</v>
       </c>
       <c r="C17" t="n">
-        <v>41.50563265940433</v>
+        <v>41</v>
       </c>
       <c r="D17" t="n">
-        <v>30.19710947158296</v>
+        <v>30</v>
       </c>
       <c r="E17" t="n">
-        <v>34.71561414850142</v>
+        <v>34</v>
       </c>
       <c r="F17" t="n">
-        <v>32.97758148196699</v>
+        <v>32</v>
       </c>
       <c r="G17" t="n">
-        <v>28.7378668712236</v>
+        <v>28</v>
       </c>
       <c r="H17" t="n">
-        <v>61.35373183100276</v>
+        <v>61</v>
       </c>
       <c r="I17" t="n">
-        <v>71.34584298681415</v>
+        <v>71</v>
       </c>
       <c r="J17" t="n">
-        <v>26.50887789075907</v>
+        <v>26</v>
       </c>
       <c r="K17" t="n">
-        <v>32.75546275286384</v>
+        <v>32</v>
       </c>
       <c r="L17" t="n">
-        <v>8.84544503083562</v>
+        <v>8</v>
       </c>
       <c r="M17" t="n">
-        <v>89.08933609939366</v>
+        <v>89</v>
       </c>
       <c r="N17" t="n">
-        <v>24.79212958345902</v>
+        <v>24</v>
       </c>
       <c r="O17" t="n">
-        <v>53.66267784029781</v>
+        <v>53</v>
       </c>
       <c r="P17" t="n">
-        <v>16.39394229109994</v>
+        <v>16</v>
       </c>
       <c r="Q17" t="n">
         <v>0</v>
       </c>
       <c r="R17" t="n">
-        <v>13.44636956565316</v>
+        <v>13</v>
       </c>
       <c r="S17" t="n">
-        <v>5.371151456393974</v>
+        <v>5</v>
       </c>
       <c r="T17" t="n">
-        <v>29.48921123151991</v>
+        <v>29</v>
       </c>
       <c r="U17" t="n">
-        <v>2.885371258267296</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18">
@@ -1614,64 +1614,64 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>19.58346306481534</v>
+        <v>19</v>
       </c>
       <c r="C18" t="n">
-        <v>10.04675171482197</v>
+        <v>10</v>
       </c>
       <c r="D18" t="n">
-        <v>6.746902998405186</v>
+        <v>6</v>
       </c>
       <c r="E18" t="n">
-        <v>7.368040317792743</v>
+        <v>7</v>
       </c>
       <c r="F18" t="n">
-        <v>10.01269413604668</v>
+        <v>10</v>
       </c>
       <c r="G18" t="n">
-        <v>8.544977673146949</v>
+        <v>8</v>
       </c>
       <c r="H18" t="n">
-        <v>12.18057984799809</v>
+        <v>12</v>
       </c>
       <c r="I18" t="n">
-        <v>19.6426930247282</v>
+        <v>19</v>
       </c>
       <c r="J18" t="n">
-        <v>6.644521418341258</v>
+        <v>6</v>
       </c>
       <c r="K18" t="n">
-        <v>6.463137570691012</v>
+        <v>6</v>
       </c>
       <c r="L18" t="n">
-        <v>2.741980715668803</v>
+        <v>2</v>
       </c>
       <c r="M18" t="n">
-        <v>16.54622947158166</v>
+        <v>16</v>
       </c>
       <c r="N18" t="n">
-        <v>4.813221780162849</v>
+        <v>4</v>
       </c>
       <c r="O18" t="n">
-        <v>7.87121270603196</v>
+        <v>7</v>
       </c>
       <c r="P18" t="n">
-        <v>3.937634374534195</v>
+        <v>3</v>
       </c>
       <c r="Q18" t="n">
-        <v>13.44636956565316</v>
+        <v>13</v>
       </c>
       <c r="R18" t="n">
         <v>0</v>
       </c>
       <c r="S18" t="n">
-        <v>1.381410950996212</v>
+        <v>1</v>
       </c>
       <c r="T18" t="n">
-        <v>11.10115034034277</v>
+        <v>11</v>
       </c>
       <c r="U18" t="n">
-        <v>0.9332032886137153</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -1681,64 +1681,64 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>45.67233265707532</v>
+        <v>45</v>
       </c>
       <c r="C19" t="n">
-        <v>17.04225531138226</v>
+        <v>17</v>
       </c>
       <c r="D19" t="n">
-        <v>13.20371190782591</v>
+        <v>13</v>
       </c>
       <c r="E19" t="n">
-        <v>10.16635119976261</v>
+        <v>10</v>
       </c>
       <c r="F19" t="n">
-        <v>13.97056726190151</v>
+        <v>13</v>
       </c>
       <c r="G19" t="n">
-        <v>9.334913483324714</v>
+        <v>9</v>
       </c>
       <c r="H19" t="n">
-        <v>12.62393291365497</v>
+        <v>12</v>
       </c>
       <c r="I19" t="n">
-        <v>11.61964733545398</v>
+        <v>11</v>
       </c>
       <c r="J19" t="n">
-        <v>23.56154612713247</v>
+        <v>23</v>
       </c>
       <c r="K19" t="n">
-        <v>13.41097756165878</v>
+        <v>13</v>
       </c>
       <c r="L19" t="n">
-        <v>4.516471886212259</v>
+        <v>4</v>
       </c>
       <c r="M19" t="n">
-        <v>22.98850868751008</v>
+        <v>22</v>
       </c>
       <c r="N19" t="n">
-        <v>8.74313941242478</v>
+        <v>8</v>
       </c>
       <c r="O19" t="n">
-        <v>8.188708509427709</v>
+        <v>8</v>
       </c>
       <c r="P19" t="n">
-        <v>15.10866647300663</v>
+        <v>15</v>
       </c>
       <c r="Q19" t="n">
-        <v>5.371151456393974</v>
+        <v>5</v>
       </c>
       <c r="R19" t="n">
-        <v>1.381410950996212</v>
+        <v>1</v>
       </c>
       <c r="S19" t="n">
         <v>0</v>
       </c>
       <c r="T19" t="n">
-        <v>4.721606764285506</v>
+        <v>4</v>
       </c>
       <c r="U19" t="n">
-        <v>1.635307985792956</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
@@ -1748,64 +1748,64 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>83.14824786265031</v>
+        <v>83</v>
       </c>
       <c r="C20" t="n">
-        <v>46.61109119060586</v>
+        <v>46</v>
       </c>
       <c r="D20" t="n">
-        <v>28.00138615746715</v>
+        <v>28</v>
       </c>
       <c r="E20" t="n">
-        <v>32.52336967366866</v>
+        <v>32</v>
       </c>
       <c r="F20" t="n">
-        <v>50.82230770753425</v>
+        <v>50</v>
       </c>
       <c r="G20" t="n">
-        <v>51.98011656689501</v>
+        <v>51</v>
       </c>
       <c r="H20" t="n">
-        <v>55.75196439482628</v>
+        <v>55</v>
       </c>
       <c r="I20" t="n">
-        <v>189.6654677537916</v>
+        <v>189</v>
       </c>
       <c r="J20" t="n">
-        <v>26.48796839735648</v>
+        <v>26</v>
       </c>
       <c r="K20" t="n">
-        <v>20.69420441642657</v>
+        <v>20</v>
       </c>
       <c r="L20" t="n">
-        <v>12.35063924385549</v>
+        <v>12</v>
       </c>
       <c r="M20" t="n">
-        <v>62.4505663961521</v>
+        <v>62</v>
       </c>
       <c r="N20" t="n">
-        <v>14.37046824364747</v>
+        <v>14</v>
       </c>
       <c r="O20" t="n">
-        <v>25.14205586302417</v>
+        <v>25</v>
       </c>
       <c r="P20" t="n">
-        <v>15.08770425834458</v>
+        <v>15</v>
       </c>
       <c r="Q20" t="n">
-        <v>29.48921123151991</v>
+        <v>29</v>
       </c>
       <c r="R20" t="n">
-        <v>11.10115034034277</v>
+        <v>11</v>
       </c>
       <c r="S20" t="n">
-        <v>4.721606764285506</v>
+        <v>4</v>
       </c>
       <c r="T20" t="n">
         <v>0</v>
       </c>
       <c r="U20" t="n">
-        <v>3.687959577928079</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21">
@@ -1815,61 +1815,61 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>19.55206696407565</v>
+        <v>19</v>
       </c>
       <c r="C21" t="n">
-        <v>8.936981748599937</v>
+        <v>8</v>
       </c>
       <c r="D21" t="n">
-        <v>5.376883589600534</v>
+        <v>5</v>
       </c>
       <c r="E21" t="n">
-        <v>4.843259864789729</v>
+        <v>4</v>
       </c>
       <c r="F21" t="n">
-        <v>16.65009348587779</v>
+        <v>16</v>
       </c>
       <c r="G21" t="n">
-        <v>8.543440697881632</v>
+        <v>8</v>
       </c>
       <c r="H21" t="n">
-        <v>6.524543999018621</v>
+        <v>6</v>
       </c>
       <c r="I21" t="n">
-        <v>8.132898353418625</v>
+        <v>8</v>
       </c>
       <c r="J21" t="n">
-        <v>7.894816085537324</v>
+        <v>7</v>
       </c>
       <c r="K21" t="n">
-        <v>3.974994251618649</v>
+        <v>3</v>
       </c>
       <c r="L21" t="n">
-        <v>8.560136261440803</v>
+        <v>8</v>
       </c>
       <c r="M21" t="n">
-        <v>9.433941642038565</v>
+        <v>9</v>
       </c>
       <c r="N21" t="n">
-        <v>2.70715868842924</v>
+        <v>2</v>
       </c>
       <c r="O21" t="n">
-        <v>3.447783344031048</v>
+        <v>3</v>
       </c>
       <c r="P21" t="n">
-        <v>4.053033450127584</v>
+        <v>4</v>
       </c>
       <c r="Q21" t="n">
-        <v>2.885371258267296</v>
+        <v>2</v>
       </c>
       <c r="R21" t="n">
-        <v>0.9332032886137153</v>
+        <v>0</v>
       </c>
       <c r="S21" t="n">
-        <v>1.635307985792956</v>
+        <v>1</v>
       </c>
       <c r="T21" t="n">
-        <v>3.687959577928079</v>
+        <v>3</v>
       </c>
       <c r="U21" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
we hebben nu een model maar hij doet nog rare dingen
</commit_message>
<xml_diff>
--- a/Code/Estimated Data/demand_2026_matrix.xlsx
+++ b/Code/Estimated Data/demand_2026_matrix.xlsx
@@ -545,28 +545,28 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="D2" t="n">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="E2" t="n">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="F2" t="n">
         <v>284</v>
       </c>
       <c r="G2" t="n">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="H2" t="n">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="I2" t="n">
         <v>234</v>
       </c>
       <c r="J2" t="n">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="K2" t="n">
         <v>166</v>
@@ -575,31 +575,31 @@
         <v>73</v>
       </c>
       <c r="M2" t="n">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="N2" t="n">
         <v>97</v>
       </c>
       <c r="O2" t="n">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="P2" t="n">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="Q2" t="n">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="R2" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="S2" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="T2" t="n">
         <v>83</v>
       </c>
       <c r="U2" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3">
@@ -609,31 +609,31 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="E3" t="n">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="F3" t="n">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="G3" t="n">
         <v>131</v>
       </c>
       <c r="H3" t="n">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="I3" t="n">
         <v>140</v>
       </c>
       <c r="J3" t="n">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="K3" t="n">
         <v>70</v>
@@ -642,19 +642,19 @@
         <v>35</v>
       </c>
       <c r="M3" t="n">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="N3" t="n">
         <v>42</v>
       </c>
       <c r="O3" t="n">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="P3" t="n">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="Q3" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="R3" t="n">
         <v>10</v>
@@ -663,10 +663,10 @@
         <v>17</v>
       </c>
       <c r="T3" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="U3" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4">
@@ -676,10 +676,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="C4" t="n">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
@@ -688,13 +688,13 @@
         <v>198</v>
       </c>
       <c r="F4" t="n">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G4" t="n">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H4" t="n">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="I4" t="n">
         <v>82</v>
@@ -709,13 +709,13 @@
         <v>19</v>
       </c>
       <c r="M4" t="n">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="N4" t="n">
         <v>37</v>
       </c>
       <c r="O4" t="n">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="P4" t="n">
         <v>85</v>
@@ -724,7 +724,7 @@
         <v>30</v>
       </c>
       <c r="R4" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="S4" t="n">
         <v>13</v>
@@ -743,10 +743,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C5" t="n">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D5" t="n">
         <v>198</v>
@@ -755,40 +755,40 @@
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G5" t="n">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H5" t="n">
         <v>318</v>
       </c>
       <c r="I5" t="n">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="J5" t="n">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="K5" t="n">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="L5" t="n">
         <v>17</v>
       </c>
       <c r="M5" t="n">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="N5" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="O5" t="n">
         <v>66</v>
       </c>
       <c r="P5" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="Q5" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="R5" t="n">
         <v>7</v>
@@ -797,10 +797,10 @@
         <v>10</v>
       </c>
       <c r="T5" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="U5" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">
@@ -813,13 +813,13 @@
         <v>284</v>
       </c>
       <c r="C6" t="n">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D6" t="n">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E6" t="n">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
@@ -840,34 +840,34 @@
         <v>43</v>
       </c>
       <c r="L6" t="n">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="M6" t="n">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="N6" t="n">
         <v>28</v>
       </c>
       <c r="O6" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="P6" t="n">
         <v>47</v>
       </c>
       <c r="Q6" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="R6" t="n">
         <v>10</v>
       </c>
       <c r="S6" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="T6" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="U6" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7">
@@ -877,16 +877,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C7" t="n">
         <v>131</v>
       </c>
       <c r="D7" t="n">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E7" t="n">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F7" t="n">
         <v>263</v>
@@ -898,43 +898,43 @@
         <v>91</v>
       </c>
       <c r="I7" t="n">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="J7" t="n">
         <v>65</v>
       </c>
       <c r="K7" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L7" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="M7" t="n">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="N7" t="n">
         <v>22</v>
       </c>
       <c r="O7" t="n">
+        <v>35</v>
+      </c>
+      <c r="P7" t="n">
         <v>34</v>
       </c>
-      <c r="P7" t="n">
-        <v>33</v>
-      </c>
       <c r="Q7" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="R7" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="S7" t="n">
         <v>9</v>
       </c>
       <c r="T7" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="U7" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8">
@@ -944,13 +944,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C8" t="n">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D8" t="n">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E8" t="n">
         <v>318</v>
@@ -974,13 +974,13 @@
         <v>75</v>
       </c>
       <c r="L8" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M8" t="n">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="N8" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="O8" t="n">
         <v>108</v>
@@ -995,13 +995,13 @@
         <v>12</v>
       </c>
       <c r="S8" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="T8" t="n">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="U8" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9">
@@ -1020,13 +1020,13 @@
         <v>82</v>
       </c>
       <c r="E9" t="n">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F9" t="n">
         <v>123</v>
       </c>
       <c r="G9" t="n">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H9" t="n">
         <v>197</v>
@@ -1038,16 +1038,16 @@
         <v>70</v>
       </c>
       <c r="K9" t="n">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L9" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M9" t="n">
         <v>186</v>
       </c>
       <c r="N9" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="O9" t="n">
         <v>70</v>
@@ -1059,13 +1059,13 @@
         <v>71</v>
       </c>
       <c r="R9" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="S9" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="T9" t="n">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="U9" t="n">
         <v>8</v>
@@ -1078,16 +1078,16 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="C10" t="n">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D10" t="n">
         <v>127</v>
       </c>
       <c r="E10" t="n">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F10" t="n">
         <v>96</v>
@@ -1108,34 +1108,34 @@
         <v>59</v>
       </c>
       <c r="L10" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M10" t="n">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="N10" t="n">
         <v>35</v>
       </c>
       <c r="O10" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="P10" t="n">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="Q10" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="R10" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="S10" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="T10" t="n">
         <v>26</v>
       </c>
       <c r="U10" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11">
@@ -1154,19 +1154,19 @@
         <v>67</v>
       </c>
       <c r="E11" t="n">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F11" t="n">
         <v>43</v>
       </c>
       <c r="G11" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H11" t="n">
         <v>75</v>
       </c>
       <c r="I11" t="n">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J11" t="n">
         <v>59</v>
@@ -1187,10 +1187,10 @@
         <v>81</v>
       </c>
       <c r="P11" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="Q11" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="R11" t="n">
         <v>6</v>
@@ -1199,10 +1199,10 @@
         <v>13</v>
       </c>
       <c r="T11" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="U11" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12">
@@ -1224,19 +1224,19 @@
         <v>17</v>
       </c>
       <c r="F12" t="n">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G12" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H12" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I12" t="n">
+        <v>29</v>
+      </c>
+      <c r="J12" t="n">
         <v>28</v>
-      </c>
-      <c r="J12" t="n">
-        <v>27</v>
       </c>
       <c r="K12" t="n">
         <v>12</v>
@@ -1251,25 +1251,25 @@
         <v>8</v>
       </c>
       <c r="O12" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="P12" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="Q12" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R12" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S12" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="T12" t="n">
         <v>12</v>
       </c>
       <c r="U12" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13">
@@ -1279,31 +1279,31 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="C13" t="n">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D13" t="n">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="E13" t="n">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="F13" t="n">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G13" t="n">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H13" t="n">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="I13" t="n">
         <v>186</v>
       </c>
       <c r="J13" t="n">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="K13" t="n">
         <v>197</v>
@@ -1315,10 +1315,10 @@
         <v>0</v>
       </c>
       <c r="N13" t="n">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="O13" t="n">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="P13" t="n">
         <v>99</v>
@@ -1327,10 +1327,10 @@
         <v>89</v>
       </c>
       <c r="R13" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="S13" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="T13" t="n">
         <v>62</v>
@@ -1355,7 +1355,7 @@
         <v>37</v>
       </c>
       <c r="E14" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F14" t="n">
         <v>28</v>
@@ -1364,10 +1364,10 @@
         <v>22</v>
       </c>
       <c r="H14" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I14" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J14" t="n">
         <v>35</v>
@@ -1379,7 +1379,7 @@
         <v>8</v>
       </c>
       <c r="M14" t="n">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="N14" t="n">
         <v>0</v>
@@ -1388,22 +1388,22 @@
         <v>55</v>
       </c>
       <c r="P14" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q14" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="R14" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="S14" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="T14" t="n">
         <v>14</v>
       </c>
       <c r="U14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15">
@@ -1413,22 +1413,22 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C15" t="n">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D15" t="n">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E15" t="n">
         <v>66</v>
       </c>
       <c r="F15" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G15" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H15" t="n">
         <v>108</v>
@@ -1437,16 +1437,16 @@
         <v>70</v>
       </c>
       <c r="J15" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K15" t="n">
         <v>81</v>
       </c>
       <c r="L15" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M15" t="n">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="N15" t="n">
         <v>55</v>
@@ -1458,10 +1458,10 @@
         <v>28</v>
       </c>
       <c r="Q15" t="n">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="R15" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="S15" t="n">
         <v>8</v>
@@ -1480,22 +1480,22 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C16" t="n">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D16" t="n">
         <v>85</v>
       </c>
       <c r="E16" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F16" t="n">
         <v>47</v>
       </c>
       <c r="G16" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H16" t="n">
         <v>52</v>
@@ -1504,19 +1504,19 @@
         <v>40</v>
       </c>
       <c r="J16" t="n">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="K16" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="L16" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="M16" t="n">
         <v>99</v>
       </c>
       <c r="N16" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O16" t="n">
         <v>28</v>
@@ -1528,7 +1528,7 @@
         <v>16</v>
       </c>
       <c r="R16" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S16" t="n">
         <v>15</v>
@@ -1547,22 +1547,22 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C17" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D17" t="n">
         <v>30</v>
       </c>
       <c r="E17" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F17" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G17" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H17" t="n">
         <v>61</v>
@@ -1571,22 +1571,22 @@
         <v>71</v>
       </c>
       <c r="J17" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K17" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="L17" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M17" t="n">
         <v>89</v>
       </c>
       <c r="N17" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O17" t="n">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="P17" t="n">
         <v>16</v>
@@ -1604,7 +1604,7 @@
         <v>29</v>
       </c>
       <c r="U17" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18">
@@ -1614,13 +1614,13 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C18" t="n">
         <v>10</v>
       </c>
       <c r="D18" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E18" t="n">
         <v>7</v>
@@ -1629,34 +1629,34 @@
         <v>10</v>
       </c>
       <c r="G18" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H18" t="n">
         <v>12</v>
       </c>
       <c r="I18" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J18" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K18" t="n">
         <v>6</v>
       </c>
       <c r="L18" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M18" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N18" t="n">
+        <v>5</v>
+      </c>
+      <c r="O18" t="n">
+        <v>8</v>
+      </c>
+      <c r="P18" t="n">
         <v>4</v>
-      </c>
-      <c r="O18" t="n">
-        <v>7</v>
-      </c>
-      <c r="P18" t="n">
-        <v>3</v>
       </c>
       <c r="Q18" t="n">
         <v>13</v>
@@ -1671,7 +1671,7 @@
         <v>11</v>
       </c>
       <c r="U18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
@@ -1681,7 +1681,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C19" t="n">
         <v>17</v>
@@ -1693,31 +1693,31 @@
         <v>10</v>
       </c>
       <c r="F19" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G19" t="n">
         <v>9</v>
       </c>
       <c r="H19" t="n">
+        <v>13</v>
+      </c>
+      <c r="I19" t="n">
         <v>12</v>
       </c>
-      <c r="I19" t="n">
-        <v>11</v>
-      </c>
       <c r="J19" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K19" t="n">
         <v>13</v>
       </c>
       <c r="L19" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M19" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N19" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="O19" t="n">
         <v>8</v>
@@ -1735,10 +1735,10 @@
         <v>0</v>
       </c>
       <c r="T19" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="U19" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20">
@@ -1751,31 +1751,31 @@
         <v>83</v>
       </c>
       <c r="C20" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D20" t="n">
         <v>28</v>
       </c>
       <c r="E20" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F20" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G20" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H20" t="n">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I20" t="n">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="J20" t="n">
         <v>26</v>
       </c>
       <c r="K20" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L20" t="n">
         <v>12</v>
@@ -1799,13 +1799,13 @@
         <v>11</v>
       </c>
       <c r="S20" t="n">
+        <v>5</v>
+      </c>
+      <c r="T20" t="n">
+        <v>0</v>
+      </c>
+      <c r="U20" t="n">
         <v>4</v>
-      </c>
-      <c r="T20" t="n">
-        <v>0</v>
-      </c>
-      <c r="U20" t="n">
-        <v>3</v>
       </c>
     </row>
     <row r="21">
@@ -1815,43 +1815,43 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C21" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D21" t="n">
         <v>5</v>
       </c>
       <c r="E21" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F21" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G21" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H21" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I21" t="n">
         <v>8</v>
       </c>
       <c r="J21" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K21" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L21" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M21" t="n">
         <v>9</v>
       </c>
       <c r="N21" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O21" t="n">
         <v>3</v>
@@ -1860,16 +1860,16 @@
         <v>4</v>
       </c>
       <c r="Q21" t="n">
+        <v>3</v>
+      </c>
+      <c r="R21" t="n">
+        <v>1</v>
+      </c>
+      <c r="S21" t="n">
         <v>2</v>
       </c>
-      <c r="R21" t="n">
-        <v>0</v>
-      </c>
-      <c r="S21" t="n">
-        <v>1</v>
-      </c>
       <c r="T21" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U21" t="n">
         <v>0</v>

</xml_diff>